<commit_message>
fix: add filters for item data import
fix blank hscode error
create design color if not exists
</commit_message>
<xml_diff>
--- a/art_collections/controllers/item_import_template.xlsx
+++ b/art_collections/controllers/item_import_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="102">
   <si>
     <t xml:space="preserve">Item Code</t>
   </si>
@@ -278,9 +278,18 @@
     <t xml:space="preserve">mauve</t>
   </si>
   <si>
+    <t xml:space="preserve">10-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-25</t>
+  </si>
+  <si>
     <t xml:space="preserve">kraft</t>
   </si>
   <si>
+    <t xml:space="preserve">0.05-0.12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Inner Carton</t>
   </si>
   <si>
@@ -291,6 +300,9 @@
   </si>
   <si>
     <t xml:space="preserve">wood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue</t>
   </si>
   <si>
     <t xml:space="preserve">dae445266b</t>
@@ -521,11 +533,11 @@
   </sheetPr>
   <dimension ref="A1:BJ6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R6" activeCellId="0" sqref="R6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AU1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="BN6" activeCellId="0" sqref="BN6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.65"/>
@@ -1150,50 +1162,52 @@
         <v>1</v>
       </c>
       <c r="V6" s="1"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="1" t="n">
-        <v>10</v>
+      <c r="W6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="Z6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AA6" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="AB6" s="1" t="n">
-        <v>0.07</v>
+      <c r="AA6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="AC6" s="1" t="n">
         <v>0.391</v>
       </c>
       <c r="AD6" s="1"/>
       <c r="AE6" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="AF6" s="1" t="n">
         <v>12</v>
       </c>
       <c r="AG6" s="1"/>
-      <c r="AH6" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="AI6" s="1" t="n">
-        <v>10</v>
+      <c r="AH6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="AJ6" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL6" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="AM6" s="1" t="n">
-        <v>1.03</v>
+        <v>87</v>
+      </c>
+      <c r="AL6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="AN6" s="1" t="n">
         <v>0.023</v>
@@ -1206,23 +1220,23 @@
         <v>23</v>
       </c>
       <c r="AR6" s="1"/>
-      <c r="AS6" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="AT6" s="1" t="n">
-        <v>17</v>
+      <c r="AS6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AT6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="AV6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AW6" s="1" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="AX6" s="1" t="n">
-        <v>2.8</v>
+      <c r="AW6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AX6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="AY6" s="1" t="n">
         <v>0.047</v>
@@ -1235,23 +1249,23 @@
         <v>48</v>
       </c>
       <c r="BC6" s="1"/>
-      <c r="BD6" s="1" t="n">
-        <v>78</v>
-      </c>
-      <c r="BE6" s="1" t="n">
-        <v>29</v>
+      <c r="BD6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BE6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="BF6" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="BG6" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BH6" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="BI6" s="1" t="n">
-        <v>3.36</v>
+      <c r="BH6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI6" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="BJ6" s="1" t="n">
         <v>0.09</v>
@@ -1283,16 +1297,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA5"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="R6 L2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="18.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="0" width="18.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.45"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,57 +1338,60 @@
         <v>5</v>
       </c>
       <c r="J1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1407,159 +1424,162 @@
         <v>10</v>
       </c>
       <c r="J2" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="L2" s="0" t="n">
         <v>555</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="0" t="s">
-        <v>88</v>
-      </c>
       <c r="N2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="O2" s="0" t="n">
-        <v>3700091767925</v>
+        <v>92</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="P2" s="0" t="n">
         <v>3700091767925</v>
       </c>
-      <c r="Q2" s="0" t="s">
-        <v>90</v>
+      <c r="Q2" s="0" t="n">
+        <v>3700091767925</v>
       </c>
       <c r="R2" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="S2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="T2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="T2" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="V2" s="0" t="n">
+      <c r="U2" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="W2" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="W2" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="X2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y2" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Z2" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="AA2" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AB2" s="0" t="n">
         <v>0.391</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q3" s="0" t="s">
-        <v>92</v>
-      </c>
       <c r="R3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="S3" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="T3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="T3" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="V3" s="0" t="n">
         <v>72</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="W3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="W3" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="X3" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y3" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z3" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="AA3" s="0" t="n">
         <v>1.03</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AB3" s="0" t="n">
         <v>0.023</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q4" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="R4" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="S4" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="T4" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="T4" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="V4" s="0" t="n">
         <v>128</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="W4" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="W4" s="0" t="s">
-        <v>86</v>
-      </c>
       <c r="X4" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y4" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Z4" s="0" t="n">
         <v>21.5</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="AA4" s="0" t="n">
         <v>2.8</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AB4" s="0" t="n">
         <v>0.047</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="Q5" s="0" t="s">
-        <v>96</v>
-      </c>
       <c r="R5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="S5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="S5" s="0" t="n">
+      <c r="T5" s="0" t="n">
         <v>48</v>
       </c>
-      <c r="T5" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="U5" s="0" t="n">
+      <c r="U5" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="V5" s="0" t="n">
         <v>78</v>
       </c>
-      <c r="V5" s="0" t="n">
+      <c r="W5" s="0" t="n">
         <v>29</v>
       </c>
-      <c r="W5" s="0" t="s">
-        <v>87</v>
-      </c>
       <c r="X5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="Y5" s="0" t="n">
+      <c r="Z5" s="0" t="n">
         <v>38</v>
       </c>
-      <c r="Z5" s="0" t="n">
+      <c r="AA5" s="0" t="n">
         <v>3.36</v>
       </c>
-      <c r="AA5" s="0" t="n">
+      <c r="AB5" s="0" t="n">
         <v>0.09</v>
       </c>
     </row>

</xml_diff>